<commit_message>
Update sample data, from xrefs to enums.
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="2440" windowWidth="25600" windowHeight="15300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1000" yWindow="340" windowWidth="33760" windowHeight="18680" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
     <sheet name="attributes" sheetId="2" r:id="rId2"/>
-    <sheet name="HOP_Gender" sheetId="3" r:id="rId3"/>
-    <sheet name="HOP_HBP" sheetId="4" r:id="rId4"/>
-    <sheet name="LifeLines_Gender" sheetId="5" r:id="rId5"/>
-    <sheet name="Prevend_Gender" sheetId="6" r:id="rId6"/>
-    <sheet name="Prevend_HT" sheetId="7" r:id="rId7"/>
-    <sheet name="Prevend" sheetId="9" r:id="rId8"/>
-    <sheet name="LifeLines" sheetId="10" r:id="rId9"/>
+    <sheet name="Prevend" sheetId="9" r:id="rId3"/>
+    <sheet name="LifeLines" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="210">
   <si>
     <t>name</t>
   </si>
@@ -113,30 +108,9 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>HOP_Gender</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>LifeLines_Gender</t>
-  </si>
-  <si>
-    <t>Prevend_Gender</t>
-  </si>
-  <si>
     <t>History of Hypertension</t>
   </si>
   <si>
-    <t>xref</t>
-  </si>
-  <si>
-    <t>HOP_HBP</t>
-  </si>
-  <si>
     <t>Height in cm</t>
   </si>
   <si>
@@ -200,9 +174,6 @@
     <t>Preven_HT_0</t>
   </si>
   <si>
-    <t>Prevend_HT</t>
-  </si>
-  <si>
     <t>Systolic Blood Pressure in mm Hg</t>
   </si>
   <si>
@@ -215,467 +186,479 @@
     <t>LifeLines_DBPa</t>
   </si>
   <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>167.5</t>
+  </si>
+  <si>
+    <t>189.5</t>
+  </si>
+  <si>
+    <t>185.5</t>
+  </si>
+  <si>
+    <t>168.0</t>
+  </si>
+  <si>
+    <t>173.0</t>
+  </si>
+  <si>
+    <t>179.5</t>
+  </si>
+  <si>
+    <t>177.0</t>
+  </si>
+  <si>
+    <t>181.0</t>
+  </si>
+  <si>
+    <t>183.0</t>
+  </si>
+  <si>
+    <t>166.0</t>
+  </si>
+  <si>
+    <t>179.0</t>
+  </si>
+  <si>
+    <t>156.0</t>
+  </si>
+  <si>
+    <t>185.0</t>
+  </si>
+  <si>
+    <t>162.0</t>
+  </si>
+  <si>
+    <t>175.0</t>
+  </si>
+  <si>
+    <t>157.5</t>
+  </si>
+  <si>
+    <t>188.0</t>
+  </si>
+  <si>
+    <t>164.5</t>
+  </si>
+  <si>
+    <t>186.0</t>
+  </si>
+  <si>
+    <t>98.0</t>
+  </si>
+  <si>
+    <t>90.0</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>71.0</t>
+  </si>
+  <si>
+    <t>86.0</t>
+  </si>
+  <si>
+    <t>90.5</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>116.5</t>
+  </si>
+  <si>
+    <t>114.0</t>
+  </si>
+  <si>
+    <t>51.0</t>
+  </si>
+  <si>
+    <t>77.0</t>
+  </si>
+  <si>
+    <t>52.0</t>
+  </si>
+  <si>
+    <t>94.0</t>
+  </si>
+  <si>
+    <t>69.0</t>
+  </si>
+  <si>
+    <t>65.0</t>
+  </si>
+  <si>
+    <t>101.5</t>
+  </si>
+  <si>
+    <t>117.5</t>
+  </si>
+  <si>
+    <t>Length (cm)</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>Prevend_WEIGH_1</t>
+  </si>
+  <si>
+    <t>Prevend_LENGT_1</t>
+  </si>
+  <si>
+    <t>160.0</t>
+  </si>
+  <si>
+    <t>81.0</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>66.0</t>
+  </si>
+  <si>
+    <t>76.0</t>
+  </si>
+  <si>
+    <t>180.0</t>
+  </si>
+  <si>
+    <t>75.0</t>
+  </si>
+  <si>
+    <t>162.5</t>
+  </si>
+  <si>
+    <t>75.5</t>
+  </si>
+  <si>
+    <t>170.5</t>
+  </si>
+  <si>
+    <t>92.0</t>
+  </si>
+  <si>
+    <t>163.5</t>
+  </si>
+  <si>
+    <t>77.5</t>
+  </si>
+  <si>
+    <t>186.5</t>
+  </si>
+  <si>
+    <t>92.5</t>
+  </si>
+  <si>
+    <t>175.5</t>
+  </si>
+  <si>
+    <t>61.5</t>
+  </si>
+  <si>
+    <t>172.0</t>
+  </si>
+  <si>
+    <t>180.5</t>
+  </si>
+  <si>
+    <t>83.5</t>
+  </si>
+  <si>
+    <t>176.5</t>
+  </si>
+  <si>
+    <t>72.0</t>
+  </si>
+  <si>
+    <t>79.0</t>
+  </si>
+  <si>
+    <t>96.0</t>
+  </si>
+  <si>
+    <t>74.0</t>
+  </si>
+  <si>
+    <t>167.0</t>
+  </si>
+  <si>
+    <t>176.0</t>
+  </si>
+  <si>
+    <t>165.0</t>
+  </si>
+  <si>
+    <t>188.5</t>
+  </si>
+  <si>
+    <t>102.5</t>
+  </si>
+  <si>
+    <t>103.0</t>
+  </si>
+  <si>
+    <t>80.0</t>
+  </si>
+  <si>
+    <t>171.0</t>
+  </si>
+  <si>
+    <t>73.0</t>
+  </si>
+  <si>
+    <t>85.0</t>
+  </si>
+  <si>
+    <t>144.0</t>
+  </si>
+  <si>
+    <t>57.0</t>
+  </si>
+  <si>
+    <t>187.0</t>
+  </si>
+  <si>
+    <t>68.5</t>
+  </si>
+  <si>
+    <t>64.5</t>
+  </si>
+  <si>
+    <t>189.0</t>
+  </si>
+  <si>
+    <t>98.5</t>
+  </si>
+  <si>
+    <t>68.0</t>
+  </si>
+  <si>
+    <t>79.5</t>
+  </si>
+  <si>
+    <t>164.0</t>
+  </si>
+  <si>
+    <t>178.0</t>
+  </si>
+  <si>
+    <t>82.0</t>
+  </si>
+  <si>
+    <t>161.5</t>
+  </si>
+  <si>
+    <t>109.0</t>
+  </si>
+  <si>
+    <t>84.0</t>
+  </si>
+  <si>
+    <t>168.5</t>
+  </si>
+  <si>
+    <t>159.5</t>
+  </si>
+  <si>
+    <t>58.5</t>
+  </si>
+  <si>
+    <t>59.0</t>
+  </si>
+  <si>
+    <t>174.5</t>
+  </si>
+  <si>
+    <t>1943-12-07T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1950-06-16T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1930-10-29T11:20:04.000+0019</t>
+  </si>
+  <si>
+    <t>1967-07-27T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1956-08-30T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1940-06-08T13:00:00.000+0200</t>
+  </si>
+  <si>
+    <t>1947-04-16T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1929-09-29T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1946-02-16T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1965-09-03T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1933-04-27T11:20:04.000+0019</t>
+  </si>
+  <si>
+    <t>1944-06-04T13:00:00.000+0200</t>
+  </si>
+  <si>
+    <t>1952-12-01T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1924-12-05T11:20:04.000+0019</t>
+  </si>
+  <si>
+    <t>1937-09-08T12:20:00.000+0120</t>
+  </si>
+  <si>
+    <t>1931-08-20T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1934-05-30T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1931-07-31T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1940-11-05T13:00:00.000+0200</t>
+  </si>
+  <si>
+    <t>1923-12-19T11:20:04.000+0019</t>
+  </si>
+  <si>
+    <t>1955-01-14T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1925-07-12T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1946-03-06T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1967-04-04T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1947-02-26T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1952-05-23T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1962-10-01T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1924-05-21T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1946-06-30T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1954-08-02T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1962-11-13T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1946-10-07T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1933-07-07T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1940-03-28T11:20:00.000+0020</t>
+  </si>
+  <si>
+    <t>1926-09-11T12:20:04.000+0119</t>
+  </si>
+  <si>
+    <t>1942-04-13T13:00:00.000+0200</t>
+  </si>
+  <si>
+    <t>1954-03-09T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1958-07-22T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1958-03-24T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1959-07-01T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1963-11-15T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1946-09-08T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1951-07-16T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1959-04-18T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1950-11-23T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1961-01-23T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1949-07-10T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1953-06-29T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>1923-05-11T11:20:04.000+0019</t>
+  </si>
+  <si>
+    <t>1949-12-14T12:00:00.000+0100</t>
+  </si>
+  <si>
+    <t>LifeLines_GENDER</t>
+  </si>
+  <si>
+    <t>enumOptions</t>
+  </si>
+  <si>
+    <t>Male,Female</t>
+  </si>
+  <si>
+    <t>No,Yes,Unknown</t>
+  </si>
+  <si>
+    <t>Yes,No</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>No</t>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>167.5</t>
-  </si>
-  <si>
-    <t>189.5</t>
-  </si>
-  <si>
-    <t>185.5</t>
-  </si>
-  <si>
-    <t>168.0</t>
-  </si>
-  <si>
-    <t>173.0</t>
-  </si>
-  <si>
-    <t>179.5</t>
-  </si>
-  <si>
-    <t>177.0</t>
-  </si>
-  <si>
-    <t>181.0</t>
-  </si>
-  <si>
-    <t>183.0</t>
-  </si>
-  <si>
-    <t>166.0</t>
-  </si>
-  <si>
-    <t>179.0</t>
-  </si>
-  <si>
-    <t>156.0</t>
-  </si>
-  <si>
-    <t>185.0</t>
-  </si>
-  <si>
-    <t>162.0</t>
-  </si>
-  <si>
-    <t>175.0</t>
-  </si>
-  <si>
-    <t>157.5</t>
-  </si>
-  <si>
-    <t>188.0</t>
-  </si>
-  <si>
-    <t>164.5</t>
-  </si>
-  <si>
-    <t>186.0</t>
-  </si>
-  <si>
-    <t>98.0</t>
-  </si>
-  <si>
-    <t>90.0</t>
-  </si>
-  <si>
-    <t>78.0</t>
-  </si>
-  <si>
-    <t>71.0</t>
-  </si>
-  <si>
-    <t>86.0</t>
-  </si>
-  <si>
-    <t>90.5</t>
-  </si>
-  <si>
-    <t>83.0</t>
-  </si>
-  <si>
-    <t>116.5</t>
-  </si>
-  <si>
-    <t>114.0</t>
-  </si>
-  <si>
-    <t>51.0</t>
-  </si>
-  <si>
-    <t>77.0</t>
-  </si>
-  <si>
-    <t>52.0</t>
-  </si>
-  <si>
-    <t>94.0</t>
-  </si>
-  <si>
-    <t>69.0</t>
-  </si>
-  <si>
-    <t>65.0</t>
-  </si>
-  <si>
-    <t>101.5</t>
-  </si>
-  <si>
-    <t>117.5</t>
-  </si>
-  <si>
-    <t>Length (cm)</t>
-  </si>
-  <si>
-    <t>Weight (kg)</t>
-  </si>
-  <si>
-    <t>Prevend_WEIGH_1</t>
-  </si>
-  <si>
-    <t>Prevend_LENGT_1</t>
-  </si>
-  <si>
-    <t>160.0</t>
-  </si>
-  <si>
-    <t>81.0</t>
-  </si>
-  <si>
-    <t>170.0</t>
-  </si>
-  <si>
-    <t>66.0</t>
-  </si>
-  <si>
-    <t>76.0</t>
-  </si>
-  <si>
-    <t>180.0</t>
-  </si>
-  <si>
-    <t>75.0</t>
-  </si>
-  <si>
-    <t>162.5</t>
-  </si>
-  <si>
-    <t>75.5</t>
-  </si>
-  <si>
-    <t>170.5</t>
-  </si>
-  <si>
-    <t>92.0</t>
-  </si>
-  <si>
-    <t>163.5</t>
-  </si>
-  <si>
-    <t>77.5</t>
-  </si>
-  <si>
-    <t>186.5</t>
-  </si>
-  <si>
-    <t>92.5</t>
-  </si>
-  <si>
-    <t>175.5</t>
-  </si>
-  <si>
-    <t>61.5</t>
-  </si>
-  <si>
-    <t>172.0</t>
-  </si>
-  <si>
-    <t>180.5</t>
-  </si>
-  <si>
-    <t>83.5</t>
-  </si>
-  <si>
-    <t>176.5</t>
-  </si>
-  <si>
-    <t>72.0</t>
-  </si>
-  <si>
-    <t>79.0</t>
-  </si>
-  <si>
-    <t>96.0</t>
-  </si>
-  <si>
-    <t>74.0</t>
-  </si>
-  <si>
-    <t>167.0</t>
-  </si>
-  <si>
-    <t>176.0</t>
-  </si>
-  <si>
-    <t>165.0</t>
-  </si>
-  <si>
-    <t>188.5</t>
-  </si>
-  <si>
-    <t>102.5</t>
-  </si>
-  <si>
-    <t>103.0</t>
-  </si>
-  <si>
-    <t>80.0</t>
-  </si>
-  <si>
-    <t>171.0</t>
-  </si>
-  <si>
-    <t>73.0</t>
-  </si>
-  <si>
-    <t>85.0</t>
-  </si>
-  <si>
-    <t>144.0</t>
-  </si>
-  <si>
-    <t>57.0</t>
-  </si>
-  <si>
-    <t>187.0</t>
-  </si>
-  <si>
-    <t>68.5</t>
-  </si>
-  <si>
-    <t>64.5</t>
-  </si>
-  <si>
-    <t>189.0</t>
-  </si>
-  <si>
-    <t>98.5</t>
-  </si>
-  <si>
-    <t>68.0</t>
-  </si>
-  <si>
-    <t>79.5</t>
-  </si>
-  <si>
-    <t>164.0</t>
-  </si>
-  <si>
-    <t>178.0</t>
-  </si>
-  <si>
-    <t>82.0</t>
-  </si>
-  <si>
-    <t>161.5</t>
-  </si>
-  <si>
-    <t>109.0</t>
-  </si>
-  <si>
-    <t>84.0</t>
-  </si>
-  <si>
-    <t>168.5</t>
-  </si>
-  <si>
-    <t>159.5</t>
-  </si>
-  <si>
-    <t>58.5</t>
-  </si>
-  <si>
-    <t>59.0</t>
-  </si>
-  <si>
-    <t>174.5</t>
-  </si>
-  <si>
-    <t>1943-12-07T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1950-06-16T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1930-10-29T11:20:04.000+0019</t>
-  </si>
-  <si>
-    <t>1967-07-27T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1956-08-30T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1940-06-08T13:00:00.000+0200</t>
-  </si>
-  <si>
-    <t>1947-04-16T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1929-09-29T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1946-02-16T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1965-09-03T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1933-04-27T11:20:04.000+0019</t>
-  </si>
-  <si>
-    <t>1944-06-04T13:00:00.000+0200</t>
-  </si>
-  <si>
-    <t>1952-12-01T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1924-12-05T11:20:04.000+0019</t>
-  </si>
-  <si>
-    <t>1937-09-08T12:20:00.000+0120</t>
-  </si>
-  <si>
-    <t>1931-08-20T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1934-05-30T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1931-07-31T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1940-11-05T13:00:00.000+0200</t>
-  </si>
-  <si>
-    <t>1923-12-19T11:20:04.000+0019</t>
-  </si>
-  <si>
-    <t>1955-01-14T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1925-07-12T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1946-03-06T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1967-04-04T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1947-02-26T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1952-05-23T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1962-10-01T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1924-05-21T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1946-06-30T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1954-08-02T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1962-11-13T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1946-10-07T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1933-07-07T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1940-03-28T11:20:00.000+0020</t>
-  </si>
-  <si>
-    <t>1926-09-11T12:20:04.000+0119</t>
-  </si>
-  <si>
-    <t>1942-04-13T13:00:00.000+0200</t>
-  </si>
-  <si>
-    <t>1954-03-09T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1958-07-22T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1958-03-24T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1959-07-01T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1963-11-15T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1946-09-08T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1951-07-16T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1959-04-18T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1950-11-23T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1961-01-23T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1949-07-10T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1953-06-29T12:00:00.000+0100</t>
-  </si>
-  <si>
-    <t>1923-05-11T11:20:04.000+0019</t>
-  </si>
-  <si>
-    <t>1949-12-14T12:00:00.000+0100</t>
-  </si>
-  <si>
     <t>Unknown</t>
-  </si>
-  <si>
-    <t>LifeLines_GENDER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -727,14 +710,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -756,7 +731,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1010,8 +985,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1029,14 +1008,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1163,6 +1139,8 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1289,6 +1267,8 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1618,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1631,19 +1611,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1669,46 +1649,6 @@
       </c>
       <c r="D4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1724,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:H31"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1738,7 +1678,7 @@
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1775,8 +1715,11 @@
       <c r="L1" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1784,7 +1727,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -1804,9 +1747,9 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1825,9 +1768,9 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1846,9 +1789,9 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1867,9 +1810,9 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -1888,21 +1831,18 @@
       </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
@@ -1911,10 +1851,13 @@
         <v>0</v>
       </c>
       <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -1923,10 +1866,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
@@ -1935,16 +1875,19 @@
         <v>0</v>
       </c>
       <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
@@ -1964,38 +1907,39 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F10" s="4"/>
       <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -2013,15 +1957,15 @@
       <c r="K11" s="3"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -2039,18 +1983,18 @@
       <c r="K12" s="3"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2065,15 +2009,15 @@
       <c r="K13" s="3"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -2091,15 +2035,15 @@
       <c r="K14" s="3"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -2117,15 +2061,15 @@
       <c r="K15" s="3"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -2145,15 +2089,15 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -2171,15 +2115,15 @@
       <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -2192,18 +2136,18 @@
       </c>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="1" t="b">
@@ -2214,9 +2158,9 @@
       </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -2225,11 +2169,9 @@
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F20" s="4"/>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
@@ -2237,23 +2179,24 @@
         <v>0</v>
       </c>
       <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="b">
         <v>1</v>
       </c>
@@ -2261,226 +2204,9 @@
         <v>0</v>
       </c>
       <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K26" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K30" s="3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" s="3"/>
+      <c r="M21" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2495,242 +2221,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>212</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F2" sqref="F2:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2745,22 +2239,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2768,19 +2262,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2788,19 +2282,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+        <v>151</v>
+      </c>
+      <c r="E3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2808,19 +2302,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+        <v>152</v>
+      </c>
+      <c r="E4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2828,19 +2322,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+        <v>153</v>
+      </c>
+      <c r="E5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2848,19 +2342,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
+        <v>154</v>
+      </c>
+      <c r="E6" t="s">
+        <v>206</v>
+      </c>
+      <c r="F6" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2868,19 +2362,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
+        <v>155</v>
+      </c>
+      <c r="E7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2888,19 +2382,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
+        <v>156</v>
+      </c>
+      <c r="E8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2908,19 +2402,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2928,19 +2422,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="E10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2948,19 +2442,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="E11" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2968,19 +2462,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2988,19 +2482,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3008,19 +2502,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>174</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
+        <v>162</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3028,19 +2522,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
+        <v>163</v>
+      </c>
+      <c r="E15" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3048,16 +2542,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="E16" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3065,19 +2562,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>177</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="E17" t="s">
+        <v>206</v>
+      </c>
+      <c r="F17" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3085,19 +2582,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
+        <v>166</v>
+      </c>
+      <c r="E18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3105,19 +2602,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>179</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="E19" t="s">
+        <v>206</v>
+      </c>
+      <c r="F19" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3125,19 +2622,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
+        <v>168</v>
+      </c>
+      <c r="E20" t="s">
+        <v>206</v>
+      </c>
+      <c r="F20" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3145,19 +2642,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
+        <v>169</v>
+      </c>
+      <c r="E21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3165,19 +2662,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="E22" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3185,19 +2682,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
+        <v>171</v>
+      </c>
+      <c r="E23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3205,19 +2702,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
+        <v>172</v>
+      </c>
+      <c r="E24" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3225,19 +2722,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3245,19 +2742,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="D26" t="s">
-        <v>186</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
+        <v>174</v>
+      </c>
+      <c r="E26" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3265,19 +2762,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D27" t="s">
-        <v>187</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
+        <v>175</v>
+      </c>
+      <c r="E27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F27" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3285,19 +2782,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
+        <v>176</v>
+      </c>
+      <c r="E28" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3305,19 +2802,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>189</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>2</v>
+        <v>177</v>
+      </c>
+      <c r="E29" t="s">
+        <v>205</v>
+      </c>
+      <c r="F29" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3325,19 +2822,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
-        <v>190</v>
-      </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3345,19 +2842,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D31" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
+        <v>179</v>
+      </c>
+      <c r="E31" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3365,19 +2862,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>192</v>
-      </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
+        <v>180</v>
+      </c>
+      <c r="E32" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3385,19 +2882,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
+        <v>181</v>
+      </c>
+      <c r="E33" t="s">
+        <v>205</v>
+      </c>
+      <c r="F33" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3405,19 +2902,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>194</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
+        <v>182</v>
+      </c>
+      <c r="E34" t="s">
+        <v>206</v>
+      </c>
+      <c r="F34" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3425,19 +2922,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="E35" t="s">
+        <v>205</v>
+      </c>
+      <c r="F35" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3445,19 +2942,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C36" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
+        <v>184</v>
+      </c>
+      <c r="E36" t="s">
+        <v>206</v>
+      </c>
+      <c r="F36" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3465,19 +2962,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>197</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
+        <v>185</v>
+      </c>
+      <c r="E37" t="s">
+        <v>205</v>
+      </c>
+      <c r="F37" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3485,19 +2982,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>198</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
+        <v>186</v>
+      </c>
+      <c r="E38" t="s">
+        <v>205</v>
+      </c>
+      <c r="F38" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3505,19 +3002,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
+        <v>187</v>
+      </c>
+      <c r="E39" t="s">
+        <v>206</v>
+      </c>
+      <c r="F39" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3525,19 +3022,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>200</v>
-      </c>
-      <c r="E40">
-        <v>2</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
+        <v>188</v>
+      </c>
+      <c r="E40" t="s">
+        <v>205</v>
+      </c>
+      <c r="F40" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3545,19 +3042,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
+        <v>189</v>
+      </c>
+      <c r="E41" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3565,19 +3062,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
-      </c>
-      <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
+        <v>190</v>
+      </c>
+      <c r="E42" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3585,19 +3082,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>203</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
+        <v>191</v>
+      </c>
+      <c r="E43" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3605,19 +3102,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>204</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
+        <v>192</v>
+      </c>
+      <c r="E44" t="s">
+        <v>205</v>
+      </c>
+      <c r="F44" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3625,19 +3122,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
+        <v>193</v>
+      </c>
+      <c r="E45" t="s">
         <v>205</v>
       </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
+      <c r="F45" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3645,19 +3142,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D46" t="s">
-        <v>206</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
+        <v>194</v>
+      </c>
+      <c r="E46" t="s">
+        <v>205</v>
+      </c>
+      <c r="F46" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3665,19 +3162,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D47" t="s">
+        <v>195</v>
+      </c>
+      <c r="E47" t="s">
+        <v>205</v>
+      </c>
+      <c r="F47" t="s">
         <v>207</v>
-      </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3685,19 +3182,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D48" t="s">
-        <v>208</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
+        <v>196</v>
+      </c>
+      <c r="E48" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3705,19 +3202,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D49" t="s">
-        <v>209</v>
-      </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
+        <v>197</v>
+      </c>
+      <c r="E49" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3725,19 +3222,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C50" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D50" t="s">
-        <v>210</v>
-      </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
+        <v>198</v>
+      </c>
+      <c r="E50" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3745,19 +3242,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="D51" t="s">
-        <v>211</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="E51" t="s">
+        <v>205</v>
+      </c>
+      <c r="F51" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3771,12 +3268,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3787,42 +3284,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>61</v>
+      <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>67</v>
+      <c r="B2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="9">
+        <v>74</v>
+      </c>
+      <c r="E2" s="8">
         <v>22160</v>
       </c>
       <c r="F2">
@@ -3836,16 +3333,16 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>68</v>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="9">
+        <v>75</v>
+      </c>
+      <c r="E3" s="8">
         <v>22402</v>
       </c>
       <c r="F3">
@@ -3859,16 +3356,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>69</v>
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="9">
+        <v>76</v>
+      </c>
+      <c r="E4" s="8">
         <v>30256</v>
       </c>
       <c r="F4">
@@ -3882,16 +3379,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>70</v>
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="9">
+        <v>77</v>
+      </c>
+      <c r="E5" s="8">
         <v>24838</v>
       </c>
       <c r="F5">
@@ -3905,16 +3402,16 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>71</v>
+      <c r="B6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="9">
+        <v>78</v>
+      </c>
+      <c r="E6" s="8">
         <v>23193</v>
       </c>
       <c r="F6">
@@ -3928,16 +3425,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>71</v>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="9">
+        <v>76</v>
+      </c>
+      <c r="E7" s="8">
         <v>21217</v>
       </c>
       <c r="F7">
@@ -3951,16 +3448,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>72</v>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E8" s="9">
+        <v>79</v>
+      </c>
+      <c r="E8" s="8">
         <v>21398</v>
       </c>
       <c r="F8">
@@ -3974,16 +3471,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>73</v>
+      <c r="B9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="9">
+        <v>80</v>
+      </c>
+      <c r="E9" s="8">
         <v>30042</v>
       </c>
       <c r="F9">
@@ -3997,16 +3494,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>74</v>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="9">
+        <v>81</v>
+      </c>
+      <c r="E10" s="8">
         <v>34151</v>
       </c>
       <c r="F10">
@@ -4020,16 +3517,16 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>75</v>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E11" s="9">
+        <v>82</v>
+      </c>
+      <c r="E11" s="8">
         <v>22160</v>
       </c>
       <c r="F11">
@@ -4043,16 +3540,16 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>76</v>
+      <c r="B12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" s="9">
+        <v>83</v>
+      </c>
+      <c r="E12" s="8">
         <v>18384</v>
       </c>
       <c r="F12">
@@ -4066,16 +3563,16 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>77</v>
+      <c r="B13" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="9">
+        <v>84</v>
+      </c>
+      <c r="E13" s="8">
         <v>23529</v>
       </c>
       <c r="F13">
@@ -4089,16 +3586,16 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>78</v>
+      <c r="B14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="9">
+        <v>85</v>
+      </c>
+      <c r="E14" s="8">
         <v>23833</v>
       </c>
       <c r="F14">
@@ -4112,16 +3609,16 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>79</v>
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" s="9">
+        <v>86</v>
+      </c>
+      <c r="E15" s="8">
         <v>21398</v>
       </c>
       <c r="F15">
@@ -4135,16 +3632,16 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>80</v>
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="9">
+        <v>87</v>
+      </c>
+      <c r="E16" s="8">
         <v>25235</v>
       </c>
       <c r="F16">
@@ -4158,16 +3655,16 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>81</v>
+      <c r="B17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" s="9">
+        <v>78</v>
+      </c>
+      <c r="E17" s="8">
         <v>24442</v>
       </c>
       <c r="F17">
@@ -4181,16 +3678,16 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>82</v>
+      <c r="B18" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="9">
+        <v>88</v>
+      </c>
+      <c r="E18" s="8">
         <v>21367</v>
       </c>
       <c r="F18">
@@ -4204,16 +3701,16 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>83</v>
+      <c r="B19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="9">
+        <v>78</v>
+      </c>
+      <c r="E19" s="8">
         <v>30682</v>
       </c>
       <c r="F19">
@@ -4227,16 +3724,16 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>84</v>
+      <c r="B20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" s="9">
+        <v>89</v>
+      </c>
+      <c r="E20" s="8">
         <v>24504</v>
       </c>
       <c r="F20">
@@ -4250,16 +3747,16 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>85</v>
+      <c r="B21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="9">
+        <v>90</v>
+      </c>
+      <c r="E21" s="8">
         <v>25235</v>
       </c>
       <c r="F21">

</xml_diff>

<commit_message>
now that xrefs can be mapped, go back to chao's original dataset
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="340" windowWidth="33760" windowHeight="18680" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6100" yWindow="2440" windowWidth="25600" windowHeight="15300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
     <sheet name="attributes" sheetId="2" r:id="rId2"/>
-    <sheet name="Prevend" sheetId="9" r:id="rId3"/>
-    <sheet name="LifeLines" sheetId="10" r:id="rId4"/>
+    <sheet name="HOP_Gender" sheetId="3" r:id="rId3"/>
+    <sheet name="HOP_HBP" sheetId="4" r:id="rId4"/>
+    <sheet name="LifeLines_Gender" sheetId="5" r:id="rId5"/>
+    <sheet name="Prevend_Gender" sheetId="6" r:id="rId6"/>
+    <sheet name="Prevend_HT" sheetId="7" r:id="rId7"/>
+    <sheet name="Prevend" sheetId="9" r:id="rId8"/>
+    <sheet name="LifeLines" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="214">
   <si>
     <t>name</t>
   </si>
@@ -108,9 +113,30 @@
     <t>Gender</t>
   </si>
   <si>
+    <t>HOP_Gender</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>LifeLines_Gender</t>
+  </si>
+  <si>
+    <t>Prevend_Gender</t>
+  </si>
+  <si>
     <t>History of Hypertension</t>
   </si>
   <si>
+    <t>xref</t>
+  </si>
+  <si>
+    <t>HOP_HBP</t>
+  </si>
+  <si>
     <t>Height in cm</t>
   </si>
   <si>
@@ -174,6 +200,9 @@
     <t>Preven_HT_0</t>
   </si>
   <si>
+    <t>Prevend_HT</t>
+  </si>
+  <si>
     <t>Systolic Blood Pressure in mm Hg</t>
   </si>
   <si>
@@ -186,6 +215,18 @@
     <t>LifeLines_DBPa</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -624,41 +665,17 @@
     <t>1949-12-14T12:00:00.000+0100</t>
   </si>
   <si>
+    <t>Unknown</t>
+  </si>
+  <si>
     <t>LifeLines_GENDER</t>
-  </si>
-  <si>
-    <t>enumOptions</t>
-  </si>
-  <si>
-    <t>Male,Female</t>
-  </si>
-  <si>
-    <t>No,Yes,Unknown</t>
-  </si>
-  <si>
-    <t>Yes,No</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -710,6 +727,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
@@ -731,7 +756,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -985,12 +1010,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1008,11 +1029,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="253">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1139,8 +1163,6 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1267,8 +1289,6 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1598,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1611,19 +1631,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1649,6 +1669,46 @@
       </c>
       <c r="D4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1664,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1678,7 +1738,7 @@
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1715,11 +1775,8 @@
       <c r="L1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1727,7 +1784,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -1747,9 +1804,9 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -1768,9 +1825,9 @@
       </c>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -1789,9 +1846,9 @@
       </c>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -1810,9 +1867,9 @@
       </c>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -1831,18 +1888,21 @@
       </c>
       <c r="K6" s="3"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="b">
         <v>1</v>
@@ -1851,13 +1911,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="M7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -1866,7 +1923,10 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>1</v>
@@ -1875,19 +1935,16 @@
         <v>0</v>
       </c>
       <c r="K8" s="3"/>
-      <c r="M8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
@@ -1907,39 +1964,38 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="M10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -1957,15 +2013,15 @@
       <c r="K11" s="3"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -1983,18 +2039,18 @@
       <c r="K12" s="3"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2009,15 +2065,15 @@
       <c r="K13" s="3"/>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>19</v>
@@ -2035,15 +2091,15 @@
       <c r="K14" s="3"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -2061,15 +2117,15 @@
       <c r="K15" s="3"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -2089,15 +2145,15 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -2115,15 +2171,15 @@
       <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -2136,18 +2192,18 @@
       </c>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="1" t="b">
@@ -2158,9 +2214,9 @@
       </c>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -2169,9 +2225,11 @@
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G20" s="1" t="b">
         <v>1</v>
       </c>
@@ -2179,34 +2237,250 @@
         <v>0</v>
       </c>
       <c r="K20" s="3"/>
-      <c r="M20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K21" s="3"/>
-      <c r="M21" t="s">
-        <v>203</v>
-      </c>
+      <c r="G22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2221,10 +2495,242 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F51"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2239,22 +2745,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2262,19 +2768,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" t="s">
-        <v>207</v>
+        <v>162</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2282,19 +2788,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F3" t="s">
-        <v>207</v>
+        <v>163</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2302,19 +2808,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F4" t="s">
-        <v>207</v>
+        <v>164</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2322,19 +2828,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F5" t="s">
-        <v>207</v>
+        <v>165</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2342,19 +2848,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F6" t="s">
-        <v>207</v>
+        <v>166</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2362,19 +2868,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" t="s">
-        <v>207</v>
+        <v>167</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2382,19 +2888,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" t="s">
-        <v>207</v>
+        <v>168</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2402,19 +2908,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F9" t="s">
-        <v>208</v>
+        <v>169</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2422,19 +2928,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" t="s">
-        <v>205</v>
-      </c>
-      <c r="F10" t="s">
-        <v>208</v>
+        <v>170</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2442,19 +2948,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" t="s">
-        <v>206</v>
-      </c>
-      <c r="F11" t="s">
-        <v>208</v>
+        <v>171</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2462,19 +2968,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" t="s">
-        <v>206</v>
-      </c>
-      <c r="F12" t="s">
-        <v>207</v>
+        <v>172</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2482,19 +2988,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
-      </c>
-      <c r="E13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F13" t="s">
-        <v>207</v>
+        <v>173</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2502,19 +3008,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>162</v>
-      </c>
-      <c r="E14" t="s">
-        <v>206</v>
-      </c>
-      <c r="F14" t="s">
-        <v>208</v>
+        <v>174</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2522,19 +3028,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E15" t="s">
-        <v>206</v>
-      </c>
-      <c r="F15" t="s">
-        <v>207</v>
+        <v>175</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2542,19 +3048,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E16" t="s">
-        <v>206</v>
-      </c>
-      <c r="F16" t="s">
-        <v>209</v>
+        <v>176</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2562,19 +3065,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
-        <v>165</v>
-      </c>
-      <c r="E17" t="s">
-        <v>206</v>
-      </c>
-      <c r="F17" t="s">
-        <v>208</v>
+        <v>177</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2582,19 +3085,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" t="s">
-        <v>206</v>
-      </c>
-      <c r="F18" t="s">
-        <v>207</v>
+        <v>178</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2602,19 +3105,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" t="s">
-        <v>206</v>
-      </c>
-      <c r="F19" t="s">
-        <v>207</v>
+        <v>179</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2622,19 +3125,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>168</v>
-      </c>
-      <c r="E20" t="s">
-        <v>206</v>
-      </c>
-      <c r="F20" t="s">
-        <v>207</v>
+        <v>180</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2642,19 +3145,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
-      </c>
-      <c r="E21" t="s">
-        <v>206</v>
-      </c>
-      <c r="F21" t="s">
-        <v>208</v>
+        <v>181</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2662,19 +3165,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
-        <v>170</v>
-      </c>
-      <c r="E22" t="s">
-        <v>205</v>
-      </c>
-      <c r="F22" t="s">
-        <v>207</v>
+        <v>182</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2682,19 +3185,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
-      </c>
-      <c r="E23" t="s">
-        <v>206</v>
-      </c>
-      <c r="F23" t="s">
-        <v>208</v>
+        <v>183</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2702,19 +3205,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
-      </c>
-      <c r="E24" t="s">
-        <v>205</v>
-      </c>
-      <c r="F24" t="s">
-        <v>208</v>
+        <v>184</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2722,19 +3225,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" t="s">
-        <v>206</v>
-      </c>
-      <c r="F25" t="s">
-        <v>208</v>
+        <v>185</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2742,19 +3245,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D26" t="s">
-        <v>174</v>
-      </c>
-      <c r="E26" t="s">
-        <v>206</v>
-      </c>
-      <c r="F26" t="s">
-        <v>207</v>
+        <v>186</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2762,19 +3265,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E27" t="s">
-        <v>205</v>
-      </c>
-      <c r="F27" t="s">
-        <v>207</v>
+        <v>187</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2782,19 +3285,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>176</v>
-      </c>
-      <c r="E28" t="s">
-        <v>206</v>
-      </c>
-      <c r="F28" t="s">
-        <v>207</v>
+        <v>188</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2802,19 +3305,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>177</v>
-      </c>
-      <c r="E29" t="s">
-        <v>205</v>
-      </c>
-      <c r="F29" t="s">
-        <v>209</v>
+        <v>189</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2822,19 +3325,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D30" t="s">
-        <v>178</v>
-      </c>
-      <c r="E30" t="s">
-        <v>206</v>
-      </c>
-      <c r="F30" t="s">
-        <v>207</v>
+        <v>190</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2842,19 +3345,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>179</v>
-      </c>
-      <c r="E31" t="s">
-        <v>205</v>
-      </c>
-      <c r="F31" t="s">
-        <v>207</v>
+        <v>191</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2862,19 +3365,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>180</v>
-      </c>
-      <c r="E32" t="s">
-        <v>206</v>
-      </c>
-      <c r="F32" t="s">
-        <v>208</v>
+        <v>192</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2882,19 +3385,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" t="s">
-        <v>205</v>
-      </c>
-      <c r="F33" t="s">
-        <v>207</v>
+        <v>193</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2902,19 +3405,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>182</v>
-      </c>
-      <c r="E34" t="s">
-        <v>206</v>
-      </c>
-      <c r="F34" t="s">
-        <v>207</v>
+        <v>194</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2922,19 +3425,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" t="s">
-        <v>205</v>
-      </c>
-      <c r="F35" t="s">
-        <v>208</v>
+        <v>195</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2942,19 +3445,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
-      </c>
-      <c r="E36" t="s">
-        <v>206</v>
-      </c>
-      <c r="F36" t="s">
-        <v>207</v>
+        <v>196</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2962,19 +3465,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="D37" t="s">
-        <v>185</v>
-      </c>
-      <c r="E37" t="s">
-        <v>205</v>
-      </c>
-      <c r="F37" t="s">
-        <v>207</v>
+        <v>197</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2982,19 +3485,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
-      </c>
-      <c r="E38" t="s">
-        <v>205</v>
-      </c>
-      <c r="F38" t="s">
-        <v>207</v>
+        <v>198</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3002,19 +3505,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D39" t="s">
-        <v>187</v>
-      </c>
-      <c r="E39" t="s">
-        <v>206</v>
-      </c>
-      <c r="F39" t="s">
-        <v>207</v>
+        <v>199</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3022,19 +3525,19 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>188</v>
-      </c>
-      <c r="E40" t="s">
-        <v>205</v>
-      </c>
-      <c r="F40" t="s">
-        <v>207</v>
+        <v>200</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3042,19 +3545,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>189</v>
-      </c>
-      <c r="E41" t="s">
-        <v>206</v>
-      </c>
-      <c r="F41" t="s">
-        <v>207</v>
+        <v>201</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3062,19 +3565,19 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>190</v>
-      </c>
-      <c r="E42" t="s">
-        <v>206</v>
-      </c>
-      <c r="F42" t="s">
-        <v>207</v>
+        <v>202</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3082,19 +3585,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>191</v>
-      </c>
-      <c r="E43" t="s">
-        <v>205</v>
-      </c>
-      <c r="F43" t="s">
-        <v>207</v>
+        <v>203</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3102,19 +3605,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>192</v>
-      </c>
-      <c r="E44" t="s">
-        <v>205</v>
-      </c>
-      <c r="F44" t="s">
-        <v>207</v>
+        <v>204</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3122,19 +3625,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>193</v>
-      </c>
-      <c r="E45" t="s">
         <v>205</v>
       </c>
-      <c r="F45" t="s">
-        <v>207</v>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3142,19 +3645,19 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="D46" t="s">
-        <v>194</v>
-      </c>
-      <c r="E46" t="s">
-        <v>205</v>
-      </c>
-      <c r="F46" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3162,19 +3665,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" t="s">
-        <v>205</v>
-      </c>
-      <c r="F47" t="s">
         <v>207</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3182,19 +3685,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
-        <v>196</v>
-      </c>
-      <c r="E48" t="s">
-        <v>205</v>
-      </c>
-      <c r="F48" t="s">
-        <v>207</v>
+        <v>208</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3202,19 +3705,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>197</v>
-      </c>
-      <c r="E49" t="s">
-        <v>205</v>
-      </c>
-      <c r="F49" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3222,19 +3725,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>198</v>
-      </c>
-      <c r="E50" t="s">
-        <v>206</v>
-      </c>
-      <c r="F50" t="s">
-        <v>207</v>
+        <v>210</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3242,19 +3745,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="D51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E51" t="s">
-        <v>205</v>
-      </c>
-      <c r="F51" t="s">
-        <v>208</v>
+        <v>211</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3268,12 +3771,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B21"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3284,42 +3787,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>53</v>
+      <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>55</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="8">
+        <v>86</v>
+      </c>
+      <c r="E2" s="9">
         <v>22160</v>
       </c>
       <c r="F2">
@@ -3333,16 +3836,16 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>56</v>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="8">
+        <v>87</v>
+      </c>
+      <c r="E3" s="9">
         <v>22402</v>
       </c>
       <c r="F3">
@@ -3356,16 +3859,16 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>57</v>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="8">
+        <v>88</v>
+      </c>
+      <c r="E4" s="9">
         <v>30256</v>
       </c>
       <c r="F4">
@@ -3379,16 +3882,16 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>58</v>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="8">
+        <v>89</v>
+      </c>
+      <c r="E5" s="9">
         <v>24838</v>
       </c>
       <c r="F5">
@@ -3402,16 +3905,16 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>59</v>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="8">
+        <v>90</v>
+      </c>
+      <c r="E6" s="9">
         <v>23193</v>
       </c>
       <c r="F6">
@@ -3425,16 +3928,16 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>59</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="8">
+        <v>88</v>
+      </c>
+      <c r="E7" s="9">
         <v>21217</v>
       </c>
       <c r="F7">
@@ -3448,16 +3951,16 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>60</v>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="8">
+        <v>91</v>
+      </c>
+      <c r="E8" s="9">
         <v>21398</v>
       </c>
       <c r="F8">
@@ -3471,16 +3974,16 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>61</v>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="8">
+        <v>92</v>
+      </c>
+      <c r="E9" s="9">
         <v>30042</v>
       </c>
       <c r="F9">
@@ -3494,16 +3997,16 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>62</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="8">
+        <v>93</v>
+      </c>
+      <c r="E10" s="9">
         <v>34151</v>
       </c>
       <c r="F10">
@@ -3517,16 +4020,16 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>205</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>63</v>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="8">
+        <v>94</v>
+      </c>
+      <c r="E11" s="9">
         <v>22160</v>
       </c>
       <c r="F11">
@@ -3540,16 +4043,16 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>205</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>64</v>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" s="8">
+        <v>95</v>
+      </c>
+      <c r="E12" s="9">
         <v>18384</v>
       </c>
       <c r="F12">
@@ -3563,16 +4066,16 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>65</v>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
-      </c>
-      <c r="E13" s="8">
+        <v>96</v>
+      </c>
+      <c r="E13" s="9">
         <v>23529</v>
       </c>
       <c r="F13">
@@ -3586,16 +4089,16 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>66</v>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="8">
+        <v>97</v>
+      </c>
+      <c r="E14" s="9">
         <v>23833</v>
       </c>
       <c r="F14">
@@ -3609,16 +4112,16 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>67</v>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="8">
+        <v>98</v>
+      </c>
+      <c r="E15" s="9">
         <v>21398</v>
       </c>
       <c r="F15">
@@ -3632,16 +4135,16 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>205</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>68</v>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="8">
+        <v>99</v>
+      </c>
+      <c r="E16" s="9">
         <v>25235</v>
       </c>
       <c r="F16">
@@ -3655,16 +4158,16 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>69</v>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="8">
+        <v>90</v>
+      </c>
+      <c r="E17" s="9">
         <v>24442</v>
       </c>
       <c r="F17">
@@ -3678,16 +4181,16 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>205</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>70</v>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" s="8">
+        <v>100</v>
+      </c>
+      <c r="E18" s="9">
         <v>21367</v>
       </c>
       <c r="F18">
@@ -3701,16 +4204,16 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>205</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>71</v>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="8">
+        <v>90</v>
+      </c>
+      <c r="E19" s="9">
         <v>30682</v>
       </c>
       <c r="F19">
@@ -3724,16 +4227,16 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>205</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>72</v>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="8">
+        <v>101</v>
+      </c>
+      <c r="E20" s="9">
         <v>24504</v>
       </c>
       <c r="F20">
@@ -3747,16 +4250,16 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>73</v>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="8">
+        <v>102</v>
+      </c>
+      <c r="E21" s="9">
         <v>25235</v>
       </c>
       <c r="F21">

</xml_diff>

<commit_message>
Edited example mapper data with descriptions so our automatic tagging tool can pick up some keywords as a test to see if ontology terms are actually mapped
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="2440" windowWidth="25600" windowHeight="15300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="217">
   <si>
     <t>name</t>
   </si>
@@ -669,6 +669,15 @@
   </si>
   <si>
     <t>LifeLines_GENDER</t>
+  </si>
+  <si>
+    <t>hospital a test description for tags</t>
+  </si>
+  <si>
+    <t>top a test description for tags</t>
+  </si>
+  <si>
+    <t>team a test description for tags</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1722,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1726,8 +1734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30:H31"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1735,6 +1743,7 @@
     <col min="1" max="1" width="34.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1789,7 +1798,9 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="b">
         <v>0</v>
@@ -1817,6 +1828,9 @@
       <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>215</v>
+      </c>
       <c r="G3" s="1" t="b">
         <v>1</v>
       </c>
@@ -1837,6 +1851,9 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>216</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
@@ -2484,7 +2501,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2529,7 +2545,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2574,7 +2589,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2619,7 +2633,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2716,7 +2729,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3762,7 +3774,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Edited test data for mapping service to work with tagging and automatic attribute mapping
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="15760" windowHeight="11300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="218">
   <si>
     <t>name</t>
   </si>
@@ -671,13 +671,16 @@
     <t>LifeLines_GENDER</t>
   </si>
   <si>
-    <t>hospital a test description for tags</t>
-  </si>
-  <si>
-    <t>top a test description for tags</t>
-  </si>
-  <si>
-    <t>team a test description for tags</t>
+    <t>Weight in kilograms</t>
+  </si>
+  <si>
+    <t>Height in centimeters</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Gender, either male or female</t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1738,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1798,9 +1801,7 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>214</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="b">
         <v>0</v>
@@ -1853,7 +1854,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>1</v>
@@ -1897,6 +1898,9 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6" t="s">
+        <v>216</v>
+      </c>
       <c r="G6" s="1" t="b">
         <v>1</v>
       </c>
@@ -1918,6 +1922,9 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
       <c r="F7" t="s">
         <v>35</v>
       </c>
@@ -1941,6 +1948,9 @@
       </c>
       <c r="D8" t="s">
         <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
       </c>
       <c r="F8" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[WIP] Implementation of category mapping editor
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="15760" windowHeight="11300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="218">
   <si>
     <t>name</t>
   </si>
@@ -1737,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2007,11 +2007,14 @@
       <c r="F10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
+      <c r="G10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2258,12 +2261,15 @@
         <v>32</v>
       </c>
       <c r="G20" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K20" s="3"/>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
@@ -2700,7 +2706,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2752,7 +2758,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3081,6 +3087,9 @@
       <c r="E16">
         <v>1</v>
       </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
@@ -3137,9 +3146,6 @@
       </c>
       <c r="E19">
         <v>1</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">

</xml_diff>

<commit_message>
Expanded example biobank data to include more then 10 genders for testing purposes
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="227">
   <si>
     <t>name</t>
   </si>
@@ -681,6 +681,33 @@
   </si>
   <si>
     <t>Gender, either male or female</t>
+  </si>
+  <si>
+    <t>Vulcan</t>
+  </si>
+  <si>
+    <t>Krogan</t>
+  </si>
+  <si>
+    <t>Asari</t>
+  </si>
+  <si>
+    <t>Martian</t>
+  </si>
+  <si>
+    <t>Jupitaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">American </t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Venusaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charizard </t>
   </si>
 </sst>
 </file>
@@ -768,8 +795,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1048,7 +1083,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="261">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1175,6 +1210,10 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1301,6 +1340,10 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1737,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView topLeftCell="B7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2615,10 +2658,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2632,23 +2675,96 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B3">
-        <v>1</v>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2659,10 +2775,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="A2" sqref="A2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2691,8 +2807,81 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>226</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Changed mapping test file
</commit_message>
<xml_diff>
--- a/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
+++ b/molgenis-data-mapper/src/test/resources/example_data_bbc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="219">
   <si>
     <t>name</t>
   </si>
@@ -683,31 +683,7 @@
     <t>Gender, either male or female</t>
   </si>
   <si>
-    <t>Vulcan</t>
-  </si>
-  <si>
-    <t>Krogan</t>
-  </si>
-  <si>
-    <t>Asari</t>
-  </si>
-  <si>
-    <t>Martian</t>
-  </si>
-  <si>
-    <t>Jupitaan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">American </t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Venusaur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charizard </t>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1780,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -2658,10 +2634,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2692,79 +2668,14 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>222</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
+        <v>9999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2775,10 +2686,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2812,76 +2723,11 @@
         <v>218</v>
       </c>
       <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>220</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>221</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>222</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>223</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>225</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>226</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
+        <v>9999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2946,7 +2792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>